<commit_message>
Tailwind : Pages 3
</commit_message>
<xml_diff>
--- a/exported.xlsx
+++ b/exported.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47" count="47">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="93" count="93">
   <x:si>
     <x:t>id</x:t>
   </x:si>
@@ -155,6 +155,144 @@
   </x:si>
   <x:si>
     <x:t>Wed Mar 22 2023 17:26:43 GMT+0530 (India Standard Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>641b538e76e5a4c58d88ef8b</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>03/01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>publishd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>piysush@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1234423423</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Female</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dhule</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Architecture</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>piyu college</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Government (affiliated) | शासकीय (संलग्न)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Karmaveer Bhaurao Patil University Satara</x:t>
+  </x:si>
+  <x:si>
+    <x:t>piyu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>piyu@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1235465476</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu Mar 23 2023 00:44:21 GMT+0530 (India Standard Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>641bbd22b596e3f660640b06</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Leadership through Outdoor Based Experiential Learning</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hello@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gondia</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fine Arts / Performance Arts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Government (autonomous) | शासकीय (स्वायत्त)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Smt. Nathibai Damodar Thakersey Women's University, Mumbai</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mvv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu Mar 23 2023 08:14:50 GMT+0530 (India Standard Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>641beb4f6cc05bd55e3e8ea3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>05/03</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2023-03-29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Through the Lens</x:t>
+  </x:si>
+  <x:si>
+    <x:t>asdasfaf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shub@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1234567890</x:t>
+  </x:si>
+  <x:si>
+    <x:t>53</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ahmednagar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Commerce</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dfsdgf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>asdasd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Punyashlok Ahilyadevi Holkar Solapur University, Solapur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>swedfswed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>asdsd@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thu Mar 23 2023 11:31:51 GMT+0530 (India Standard Time)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -662,6 +800,207 @@
         <x:v>46</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" spans="1:26">
+      <x:c r="A3" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="S3" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="T3" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="U3" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="V3" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="W3" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="X3" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="Y3" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="Z3" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:26">
+      <x:c r="A4" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="N4" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="S4" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="T4" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="U4" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="V4" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="W4" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="X4" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="Y4" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="Z4" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:26">
+      <x:c r="A5" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="S5" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="T5" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="U5" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="V5" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="W5" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="X5" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="Y5" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="Z5" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>